<commit_message>
updated skillsets, ram and rtm
</commit_message>
<xml_diff>
--- a/MGMT/PLAN/PP/WORK IN PROGRESS/skillsets.xlsx
+++ b/MGMT/PLAN/PP/WORK IN PROGRESS/skillsets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmb/learning/MTECH/SE25PT7SERIS/MGMT/PLAN/PP/WORK IN PROGRESS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF8E55D-DD69-2944-A63A-5C1F56A15913}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2EC219-D500-EA4B-9100-88ACDD5AFB8A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -303,18 +303,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -331,13 +319,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,7 +683,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -694,51 +694,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="4" t="s">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="4" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3" t="s">
+      <c r="G1" s="22"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
       <c r="O1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="7" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="5" t="s">
         <v>29</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -767,25 +767,25 @@
       <c r="A3" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="10">
-        <v>7</v>
-      </c>
-      <c r="D3" s="11">
-        <v>7</v>
-      </c>
-      <c r="E3" s="12">
+      <c r="C3" s="6">
+        <v>7</v>
+      </c>
+      <c r="D3" s="7">
+        <v>7</v>
+      </c>
+      <c r="E3" s="8">
         <v>8</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="6">
         <v>8</v>
       </c>
-      <c r="G3" s="16">
-        <v>9</v>
-      </c>
-      <c r="H3" s="12">
+      <c r="G3" s="12">
+        <v>9</v>
+      </c>
+      <c r="H3" s="8">
         <v>9</v>
       </c>
       <c r="I3">
@@ -797,25 +797,25 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="20"/>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="10">
-        <v>2</v>
-      </c>
-      <c r="D4" s="11">
-        <v>2</v>
-      </c>
-      <c r="E4" s="12">
+      <c r="C4" s="6">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7">
+        <v>2</v>
+      </c>
+      <c r="E4" s="8">
         <v>3</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="6">
         <v>4</v>
       </c>
-      <c r="G4" s="16">
-        <v>7</v>
-      </c>
-      <c r="H4" s="12">
+      <c r="G4" s="12">
+        <v>7</v>
+      </c>
+      <c r="H4" s="8">
         <v>7</v>
       </c>
       <c r="I4">
@@ -827,49 +827,49 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="20"/>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="10">
-        <v>2</v>
-      </c>
-      <c r="D5" s="11">
-        <v>2</v>
-      </c>
-      <c r="E5" s="12">
+      <c r="C5" s="6">
+        <v>2</v>
+      </c>
+      <c r="D5" s="7">
+        <v>2</v>
+      </c>
+      <c r="E5" s="8">
         <v>3</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="6">
         <v>0</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="12">
         <v>0</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="20"/>
-      <c r="B6" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="10">
-        <v>2</v>
-      </c>
-      <c r="D6" s="11">
-        <v>2</v>
-      </c>
-      <c r="E6" s="12">
+      <c r="B6" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="7">
+        <v>2</v>
+      </c>
+      <c r="E6" s="8">
         <v>3</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="6">
         <v>1</v>
       </c>
-      <c r="G6" s="16">
+      <c r="G6" s="12">
         <v>4</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="8">
         <v>6</v>
       </c>
       <c r="I6">
@@ -881,25 +881,25 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="20"/>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="10">
-        <v>2</v>
-      </c>
-      <c r="D7" s="11">
-        <v>2</v>
-      </c>
-      <c r="E7" s="12">
+      <c r="C7" s="6">
+        <v>2</v>
+      </c>
+      <c r="D7" s="7">
+        <v>2</v>
+      </c>
+      <c r="E7" s="8">
         <v>3</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="6">
         <v>1</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="12">
         <v>3</v>
       </c>
-      <c r="H7" s="12"/>
+      <c r="H7" s="8"/>
       <c r="I7">
         <v>3</v>
       </c>
@@ -909,43 +909,43 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="20"/>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="10">
+      <c r="C8" s="6"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="6">
         <v>1</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8" s="12">
         <v>3</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="8">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="20"/>
-      <c r="B9" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="10">
+      <c r="B9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="6">
         <v>1</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="7">
         <v>1</v>
       </c>
-      <c r="E9" s="12">
-        <v>2</v>
-      </c>
-      <c r="F9" s="10">
+      <c r="E9" s="8">
+        <v>2</v>
+      </c>
+      <c r="F9" s="6">
         <v>0</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="12">
         <v>4</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="8">
         <v>7</v>
       </c>
       <c r="I9">
@@ -957,25 +957,25 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="20"/>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="6">
         <v>1</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="7">
         <v>1</v>
       </c>
-      <c r="E10" s="12">
-        <v>2</v>
-      </c>
-      <c r="F10" s="10">
+      <c r="E10" s="8">
+        <v>2</v>
+      </c>
+      <c r="F10" s="6">
         <v>5</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="12">
         <v>5</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="8">
         <v>5</v>
       </c>
       <c r="I10">
@@ -987,25 +987,25 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="20"/>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="6">
         <v>4</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="7">
         <v>4</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="8">
         <v>5</v>
       </c>
-      <c r="F11" s="10">
-        <v>7</v>
-      </c>
-      <c r="G11" s="16">
-        <v>7</v>
-      </c>
-      <c r="H11" s="12">
+      <c r="F11" s="6">
+        <v>7</v>
+      </c>
+      <c r="G11" s="12">
+        <v>7</v>
+      </c>
+      <c r="H11" s="8">
         <v>7</v>
       </c>
       <c r="I11">
@@ -1017,25 +1017,25 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="20"/>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="10">
-        <v>2</v>
-      </c>
-      <c r="D12" s="11">
-        <v>2</v>
-      </c>
-      <c r="E12" s="12">
+      <c r="C12" s="6">
+        <v>2</v>
+      </c>
+      <c r="D12" s="7">
+        <v>2</v>
+      </c>
+      <c r="E12" s="8">
         <v>3</v>
       </c>
-      <c r="F12" s="10">
-        <v>7</v>
-      </c>
-      <c r="G12" s="16">
-        <v>7</v>
-      </c>
-      <c r="H12" s="12">
+      <c r="F12" s="6">
+        <v>7</v>
+      </c>
+      <c r="G12" s="12">
+        <v>7</v>
+      </c>
+      <c r="H12" s="8">
         <v>7</v>
       </c>
       <c r="I12">
@@ -1047,205 +1047,205 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="20"/>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="6">
         <v>1</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="7">
         <v>1</v>
       </c>
-      <c r="E13" s="12">
-        <v>2</v>
-      </c>
-      <c r="F13" s="10">
-        <v>7</v>
-      </c>
-      <c r="G13" s="16">
-        <v>7</v>
-      </c>
-      <c r="H13" s="12">
+      <c r="E13" s="8">
+        <v>2</v>
+      </c>
+      <c r="F13" s="6">
+        <v>7</v>
+      </c>
+      <c r="G13" s="12">
+        <v>7</v>
+      </c>
+      <c r="H13" s="8">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="20"/>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="10">
-        <v>2</v>
-      </c>
-      <c r="D14" s="11">
-        <v>2</v>
-      </c>
-      <c r="E14" s="12">
+      <c r="C14" s="6">
+        <v>2</v>
+      </c>
+      <c r="D14" s="7">
+        <v>2</v>
+      </c>
+      <c r="E14" s="8">
         <v>3</v>
       </c>
-      <c r="F14" s="10">
-        <v>7</v>
-      </c>
-      <c r="G14" s="16">
-        <v>7</v>
-      </c>
-      <c r="H14" s="12">
+      <c r="F14" s="6">
+        <v>7</v>
+      </c>
+      <c r="G14" s="12">
+        <v>7</v>
+      </c>
+      <c r="H14" s="8">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="20"/>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="10">
-        <v>2</v>
-      </c>
-      <c r="D15" s="11">
-        <v>2</v>
-      </c>
-      <c r="E15" s="12">
+      <c r="C15" s="6">
+        <v>2</v>
+      </c>
+      <c r="D15" s="7">
+        <v>2</v>
+      </c>
+      <c r="E15" s="8">
         <v>3</v>
       </c>
-      <c r="F15" s="10">
-        <v>7</v>
-      </c>
-      <c r="G15" s="16">
-        <v>7</v>
-      </c>
-      <c r="H15" s="12">
+      <c r="F15" s="6">
+        <v>7</v>
+      </c>
+      <c r="G15" s="12">
+        <v>7</v>
+      </c>
+      <c r="H15" s="8">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="20"/>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="6">
         <v>5</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="7">
         <v>5</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="8">
         <v>5</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="6">
         <v>8</v>
       </c>
-      <c r="G16" s="16">
+      <c r="G16" s="12">
         <v>8</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="8">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="20"/>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="10">
-        <v>7</v>
-      </c>
-      <c r="D17" s="11">
-        <v>7</v>
-      </c>
-      <c r="E17" s="12">
+      <c r="C17" s="6">
+        <v>7</v>
+      </c>
+      <c r="D17" s="7">
+        <v>7</v>
+      </c>
+      <c r="E17" s="8">
         <v>8</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="6">
         <v>1</v>
       </c>
-      <c r="G17" s="16">
+      <c r="G17" s="12">
         <v>1</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="20"/>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="10">
-        <v>0</v>
-      </c>
-      <c r="D18" s="16">
-        <v>0</v>
-      </c>
-      <c r="E18" s="12">
-        <v>0</v>
-      </c>
-      <c r="F18" s="10">
-        <v>2</v>
-      </c>
-      <c r="G18" s="16">
+      <c r="C18" s="6">
+        <v>2</v>
+      </c>
+      <c r="D18" s="12">
+        <v>3</v>
+      </c>
+      <c r="E18" s="8">
         <v>4</v>
       </c>
-      <c r="H18" s="12">
+      <c r="F18" s="6">
+        <v>2</v>
+      </c>
+      <c r="G18" s="12">
+        <v>4</v>
+      </c>
+      <c r="H18" s="8">
         <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="21"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="12"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="8"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="6">
         <v>8</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="7">
         <v>8</v>
       </c>
-      <c r="E20" s="12">
-        <v>9</v>
-      </c>
-      <c r="F20" s="10">
-        <v>7</v>
-      </c>
-      <c r="G20" s="16">
-        <v>7</v>
-      </c>
-      <c r="H20" s="12">
+      <c r="E20" s="8">
+        <v>9</v>
+      </c>
+      <c r="F20" s="6">
+        <v>7</v>
+      </c>
+      <c r="G20" s="12">
+        <v>7</v>
+      </c>
+      <c r="H20" s="8">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="20"/>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="10">
-        <v>9</v>
-      </c>
-      <c r="D21" s="11">
-        <v>9</v>
-      </c>
-      <c r="E21" s="12">
-        <v>9</v>
-      </c>
-      <c r="F21" s="10">
-        <v>9</v>
-      </c>
-      <c r="G21" s="16">
-        <v>9</v>
-      </c>
-      <c r="H21" s="12">
+      <c r="C21" s="6">
+        <v>9</v>
+      </c>
+      <c r="D21" s="7">
+        <v>9</v>
+      </c>
+      <c r="E21" s="8">
+        <v>9</v>
+      </c>
+      <c r="F21" s="6">
+        <v>9</v>
+      </c>
+      <c r="G21" s="12">
+        <v>9</v>
+      </c>
+      <c r="H21" s="8">
         <v>9</v>
       </c>
       <c r="I21">
@@ -1257,83 +1257,83 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="20"/>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="6">
         <v>8</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="7">
         <v>8</v>
       </c>
-      <c r="E22" s="12">
-        <v>9</v>
-      </c>
-      <c r="F22" s="10">
-        <v>9</v>
-      </c>
-      <c r="G22" s="16">
-        <v>9</v>
-      </c>
-      <c r="H22" s="12">
+      <c r="E22" s="8">
+        <v>9</v>
+      </c>
+      <c r="F22" s="6">
+        <v>9</v>
+      </c>
+      <c r="G22" s="12">
+        <v>9</v>
+      </c>
+      <c r="H22" s="8">
         <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="21"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="12"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="21"/>
-      <c r="B24" s="18" t="s">
+      <c r="A24" s="16"/>
+      <c r="B24" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="6">
         <v>8</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="7">
         <v>8</v>
       </c>
-      <c r="E24" s="12">
-        <v>9</v>
-      </c>
-      <c r="F24" s="10">
+      <c r="E24" s="8">
+        <v>9</v>
+      </c>
+      <c r="F24" s="6">
         <v>4</v>
       </c>
-      <c r="G24" s="16">
+      <c r="G24" s="12">
         <v>5</v>
       </c>
-      <c r="H24" s="12">
+      <c r="H24" s="8">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="19" t="s">
+      <c r="A25" s="17"/>
+      <c r="B25" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="13">
+      <c r="C25" s="9">
         <v>8</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="10">
         <v>8</v>
       </c>
-      <c r="E25" s="15">
-        <v>9</v>
-      </c>
-      <c r="F25" s="13">
+      <c r="E25" s="11">
+        <v>9</v>
+      </c>
+      <c r="F25" s="9">
         <v>3</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="10">
         <v>4</v>
       </c>
-      <c r="H25" s="15">
+      <c r="H25" s="11">
         <v>4</v>
       </c>
     </row>
@@ -1408,39 +1408,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="4ea5e6aa-6838-422c-a4a7-68563e031b96">
-      <UserInfo>
-        <DisplayName>MTECH-SE PT-7</DisplayName>
-        <AccountId>7</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Treza Bawm Win</DisplayName>
-        <AccountId>14</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kaung Myat Bo</DisplayName>
-        <AccountId>17</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005B49AD9B331C4641B4046595A2039F92" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f9b45159473b27e044485c23f55d4df5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="061dbba2-bf6f-42a7-92c2-825cebdcde53" xmlns:ns3="4ea5e6aa-6838-422c-a4a7-68563e031b96" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="76cbf2ca174bf1483c4c5692bb00f5ba" ns2:_="" ns3:_="">
     <xsd:import namespace="061dbba2-bf6f-42a7-92c2-825cebdcde53"/>
@@ -1605,25 +1572,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1372794-2848-40D0-8759-186E2A57CF9C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4ea5e6aa-6838-422c-a4a7-68563e031b96"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA10A8D5-7A56-491A-B32C-ED2A0C63273C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="4ea5e6aa-6838-422c-a4a7-68563e031b96">
+      <UserInfo>
+        <DisplayName>MTECH-SE PT-7</DisplayName>
+        <AccountId>7</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Treza Bawm Win</DisplayName>
+        <AccountId>14</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kaung Myat Bo</DisplayName>
+        <AccountId>17</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21DC2B48-225D-4F29-AC2C-86F50C48D6A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1640,4 +1622,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA10A8D5-7A56-491A-B32C-ED2A0C63273C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1372794-2848-40D0-8759-186E2A57CF9C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4ea5e6aa-6838-422c-a4a7-68563e031b96"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>